<commit_message>
debugged the warming-up period
</commit_message>
<xml_diff>
--- a/parameter_study/parameter_v2.xlsx
+++ b/parameter_study/parameter_v2.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Ryoko and Hilary\SMSigxModel\analysis\parameter_study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83607195-64DD-4083-9F68-7EEF8AB98A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D56BCB-9160-47DD-8690-749674C8E23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{C2B8906E-1C3B-4D84-9FF7-ACBD70084FC6}"/>
-    <workbookView minimized="1" xWindow="7590" yWindow="5430" windowWidth="15375" windowHeight="7950" activeTab="1" xr2:uid="{92903A29-01B9-41CB-A24E-F02EE5763081}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{C2B8906E-1C3B-4D84-9FF7-ACBD70084FC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Definition &amp; analysis design" sheetId="1" r:id="rId1"/>
@@ -341,10 +340,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>?</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Sensitivity</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -982,6 +977,10 @@
   </si>
   <si>
     <t>Calculated using streamflow shapefile given by Hilary https://www.notion.so/raraki/Drainage-density-fb8efbeb5d064e91845399729dc44fed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GLUE</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1753,13 +1752,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T40"/>
+  <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="I14" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -1775,111 +1774,115 @@
     <col min="10" max="10" width="16.625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="1" customWidth="1"/>
     <col min="12" max="12" width="15.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.25" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17" style="1" customWidth="1"/>
-    <col min="16" max="16" width="26.75" style="1" customWidth="1"/>
-    <col min="17" max="17" width="16.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9" style="1"/>
-    <col min="19" max="19" width="13.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="1"/>
+    <col min="13" max="14" width="21.25" style="1" customWidth="1"/>
+    <col min="15" max="15" width="20.875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17" style="1" customWidth="1"/>
+    <col min="17" max="17" width="26.75" style="1" customWidth="1"/>
+    <col min="18" max="18" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" style="1"/>
+    <col min="20" max="20" width="13.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" ht="18.75" customHeight="1">
+    <row r="1" spans="1:21" s="5" customFormat="1" ht="18.75" customHeight="1">
       <c r="A1" s="59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
       <c r="D1" s="60"/>
       <c r="E1" s="61"/>
       <c r="F1" s="59" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G1" s="63"/>
       <c r="H1" s="63"/>
       <c r="I1" s="64"/>
       <c r="J1" s="62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K1" s="60"/>
       <c r="L1" s="60"/>
       <c r="M1" s="60"/>
       <c r="N1" s="60"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="62" t="s">
+        <v>88</v>
+      </c>
       <c r="R1" s="60"/>
       <c r="S1" s="60"/>
-      <c r="T1" s="61"/>
-    </row>
-    <row r="2" spans="1:20" s="5" customFormat="1" ht="33">
+      <c r="T1" s="60"/>
+      <c r="U1" s="61"/>
+    </row>
+    <row r="2" spans="1:21" s="5" customFormat="1" ht="33">
       <c r="A2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>85</v>
-      </c>
       <c r="J2" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="L2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q2" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="N2" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O2" s="8" t="s">
+      <c r="R2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="P2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="8" t="s">
+      <c r="U2" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="T2" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" s="2" customFormat="1" ht="99">
+    </row>
+    <row r="3" spans="1:21" s="2" customFormat="1" ht="99">
       <c r="A3" s="57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>3</v>
@@ -1888,10 +1891,10 @@
         <v>19</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>54</v>
@@ -1903,10 +1906,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K3" s="19">
         <f>'Lit review on WRF-Hydro'!G3</f>
@@ -1920,29 +1923,30 @@
         <f>'Lit review on WRF-Hydro'!I3</f>
         <v>15</v>
       </c>
-      <c r="N3" s="11"/>
+      <c r="N3" s="19"/>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
-      <c r="Q3" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="R3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11" t="s">
+        <v>90</v>
+      </c>
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
-    </row>
-    <row r="4" spans="1:20" s="2" customFormat="1" ht="49.5">
+      <c r="U3" s="11"/>
+    </row>
+    <row r="4" spans="1:21" s="2" customFormat="1" ht="49.5">
       <c r="A4" s="65"/>
       <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>54</v>
@@ -1954,10 +1958,10 @@
         <v>0</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K4" s="14">
         <f>'Lit review on WRF-Hydro'!G9</f>
@@ -1971,27 +1975,28 @@
         <f>'Lit review on WRF-Hydro'!I9</f>
         <v>2.4499999999999999E-5</v>
       </c>
-      <c r="N4" s="11"/>
+      <c r="N4" s="14"/>
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
-    </row>
-    <row r="5" spans="1:20" s="2" customFormat="1" ht="33">
+      <c r="U4" s="11"/>
+    </row>
+    <row r="5" spans="1:21" s="2" customFormat="1" ht="33">
       <c r="A5" s="65"/>
       <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>54</v>
@@ -2006,7 +2011,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K5" s="20">
         <f>'Lit review on WRF-Hydro'!G15</f>
@@ -2020,42 +2025,43 @@
         <f>'Lit review on WRF-Hydro'!I15</f>
         <v>1</v>
       </c>
-      <c r="N5" s="11"/>
+      <c r="N5" s="20"/>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
       <c r="S5" s="11"/>
       <c r="T5" s="11"/>
-    </row>
-    <row r="6" spans="1:20" s="2" customFormat="1" ht="49.5">
+      <c r="U5" s="11"/>
+    </row>
+    <row r="6" spans="1:21" s="2" customFormat="1" ht="49.5">
       <c r="A6" s="65"/>
       <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>54</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H6" s="11">
         <v>0</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K6" s="11">
         <f>'Lit review on WRF-Hydro'!G20</f>
@@ -2076,20 +2082,21 @@
       <c r="R6" s="11"/>
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
-    </row>
-    <row r="7" spans="1:20" s="2" customFormat="1" ht="99">
+      <c r="U6" s="11"/>
+    </row>
+    <row r="7" spans="1:21" s="2" customFormat="1" ht="99">
       <c r="A7" s="65"/>
       <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>54</v>
@@ -2098,13 +2105,13 @@
         <v>19</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I7" s="11">
         <v>1</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K7" s="11">
         <v>0.5</v>
@@ -2122,20 +2129,21 @@
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
-    </row>
-    <row r="8" spans="1:20" s="2" customFormat="1" ht="99">
+      <c r="U7" s="11"/>
+    </row>
+    <row r="8" spans="1:21" s="2" customFormat="1" ht="99">
       <c r="A8" s="65"/>
       <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>41</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>54</v>
@@ -2147,10 +2155,10 @@
         <v>0</v>
       </c>
       <c r="I8" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="K8" s="11">
         <v>0.35</v>
@@ -2168,20 +2176,21 @@
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
       <c r="T8" s="11"/>
-    </row>
-    <row r="9" spans="1:20" s="2" customFormat="1" ht="99">
+      <c r="U8" s="11"/>
+    </row>
+    <row r="9" spans="1:21" s="2" customFormat="1" ht="99">
       <c r="A9" s="65"/>
       <c r="B9" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>54</v>
@@ -2196,7 +2205,7 @@
         <v>0.33</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K9" s="11">
         <v>0.33</v>
@@ -2216,8 +2225,9 @@
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
       <c r="T9" s="11"/>
-    </row>
-    <row r="10" spans="1:20" s="17" customFormat="1" ht="82.5">
+      <c r="U9" s="11"/>
+    </row>
+    <row r="10" spans="1:21" s="17" customFormat="1" ht="82.5">
       <c r="A10" s="65"/>
       <c r="B10" s="15" t="s">
         <v>51</v>
@@ -2226,16 +2236,16 @@
         <v>19</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>53</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>19</v>
@@ -2262,32 +2272,33 @@
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
       <c r="T10" s="16"/>
-    </row>
-    <row r="11" spans="1:20" s="2" customFormat="1" ht="99">
+      <c r="U10" s="16"/>
+    </row>
+    <row r="11" spans="1:21" s="2" customFormat="1" ht="99">
       <c r="A11" s="65"/>
       <c r="B11" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>53</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H11" s="16">
         <v>0</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J11" s="16" t="s">
         <v>19</v>
@@ -2301,15 +2312,16 @@
       <c r="M11" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="11"/>
+      <c r="N11" s="16"/>
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
       <c r="T11" s="11"/>
-    </row>
-    <row r="12" spans="1:20" s="17" customFormat="1" ht="82.5">
+      <c r="U11" s="11"/>
+    </row>
+    <row r="12" spans="1:21" s="17" customFormat="1" ht="82.5">
       <c r="A12" s="65"/>
       <c r="B12" s="15" t="s">
         <v>50</v>
@@ -2318,16 +2330,16 @@
         <v>19</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>53</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>19</v>
@@ -2354,26 +2366,27 @@
       <c r="R12" s="16"/>
       <c r="S12" s="16"/>
       <c r="T12" s="16"/>
-    </row>
-    <row r="13" spans="1:20" s="17" customFormat="1" ht="99">
+      <c r="U12" s="16"/>
+    </row>
+    <row r="13" spans="1:21" s="17" customFormat="1" ht="99">
       <c r="A13" s="65"/>
       <c r="B13" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>53</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H13" s="16" t="s">
         <v>19</v>
@@ -2400,26 +2413,27 @@
       <c r="R13" s="16"/>
       <c r="S13" s="16"/>
       <c r="T13" s="16"/>
-    </row>
-    <row r="14" spans="1:20" s="3" customFormat="1" ht="148.5">
+      <c r="U13" s="16"/>
+    </row>
+    <row r="14" spans="1:21" s="3" customFormat="1" ht="148.5">
       <c r="A14" s="65"/>
       <c r="B14" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="D14" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D14" s="16" t="s">
-        <v>127</v>
-      </c>
       <c r="E14" s="55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>53</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H14" s="16">
         <v>0</v>
@@ -2428,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K14" s="16">
         <v>1.4350000000000001E-3</v>
@@ -2439,18 +2453,19 @@
       <c r="M14" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="N14" s="11"/>
+      <c r="N14" s="16"/>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
       <c r="T14" s="11"/>
-    </row>
-    <row r="15" spans="1:20" s="3" customFormat="1" ht="49.5">
+      <c r="U14" s="11"/>
+    </row>
+    <row r="15" spans="1:21" s="3" customFormat="1" ht="49.5">
       <c r="A15" s="65"/>
       <c r="B15" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>19</v>
@@ -2459,7 +2474,7 @@
         <v>43</v>
       </c>
       <c r="E15" s="56" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>54</v>
@@ -2471,10 +2486,10 @@
         <v>0</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K15" s="11">
         <f>'Lit review on WRF-Hydro'!G26</f>
@@ -2495,14 +2510,15 @@
       <c r="R15" s="11"/>
       <c r="S15" s="11"/>
       <c r="T15" s="11"/>
-    </row>
-    <row r="16" spans="1:20" s="2" customFormat="1" ht="33">
+      <c r="U15" s="11"/>
+    </row>
+    <row r="16" spans="1:21" s="2" customFormat="1" ht="33">
       <c r="A16" s="65"/>
       <c r="B16" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>44</v>
@@ -2520,10 +2536,10 @@
         <v>0</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K16" s="11">
         <f>'Lit review on WRF-Hydro'!G29</f>
@@ -2544,11 +2560,12 @@
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
       <c r="T16" s="11"/>
-    </row>
-    <row r="17" spans="1:20" s="2" customFormat="1" ht="66">
+      <c r="U16" s="11"/>
+    </row>
+    <row r="17" spans="1:21" s="2" customFormat="1" ht="66">
       <c r="A17" s="58"/>
       <c r="B17" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>19</v>
@@ -2557,7 +2574,7 @@
         <v>52</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>54</v>
@@ -2572,43 +2589,44 @@
         <v>1</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K17" s="20">
         <f>'Lit review on WRF-Hydro'!G32</f>
-        <v>0.27777777777777779</v>
+        <v>0.625</v>
       </c>
       <c r="L17" s="20">
         <f>'Lit review on WRF-Hydro'!H32</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="M17" s="20">
         <f>'Lit review on WRF-Hydro'!I32</f>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="N17" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="N17" s="20"/>
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
-    </row>
-    <row r="18" spans="1:20" s="3" customFormat="1" ht="49.5">
+      <c r="U17" s="11"/>
+    </row>
+    <row r="18" spans="1:21" s="3" customFormat="1" ht="49.5">
       <c r="A18" s="57" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>39</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>54</v>
@@ -2620,22 +2638,22 @@
         <v>0</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K18" s="11">
         <f>'Lit review on WRF-Hydro'!G35</f>
-        <v>0.05</v>
+        <v>50</v>
       </c>
       <c r="L18" s="11">
         <f>'Lit review on WRF-Hydro'!H35</f>
-        <v>0.01</v>
+        <v>10</v>
       </c>
       <c r="M18" s="11">
         <f>'Lit review on WRF-Hydro'!I35</f>
-        <v>0.25</v>
+        <v>250</v>
       </c>
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
@@ -2644,20 +2662,21 @@
       <c r="R18" s="11"/>
       <c r="S18" s="11"/>
       <c r="T18" s="11"/>
-    </row>
-    <row r="19" spans="1:20" s="3" customFormat="1" ht="82.5">
+      <c r="U18" s="11"/>
+    </row>
+    <row r="19" spans="1:21" s="3" customFormat="1" ht="82.5">
       <c r="A19" s="65"/>
       <c r="B19" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>54</v>
@@ -2669,10 +2688,10 @@
         <v>0</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K19" s="11">
         <f>'Lit review on WRF-Hydro'!G40</f>
@@ -2693,8 +2712,9 @@
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
       <c r="T19" s="11"/>
-    </row>
-    <row r="20" spans="1:20" s="3" customFormat="1" ht="99">
+      <c r="U19" s="11"/>
+    </row>
+    <row r="20" spans="1:21" s="3" customFormat="1" ht="99">
       <c r="A20" s="58"/>
       <c r="B20" s="10" t="s">
         <v>12</v>
@@ -2706,7 +2726,7 @@
         <v>49</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>54</v>
@@ -2718,10 +2738,10 @@
         <v>0</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K20" s="11">
         <f>'Lit review on WRF-Hydro'!G44</f>
@@ -2742,10 +2762,11 @@
       <c r="R20" s="11"/>
       <c r="S20" s="11"/>
       <c r="T20" s="11"/>
-    </row>
-    <row r="21" spans="1:20" s="2" customFormat="1" ht="66">
+      <c r="U20" s="11"/>
+    </row>
+    <row r="21" spans="1:21" s="2" customFormat="1" ht="66">
       <c r="A21" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>45</v>
@@ -2754,10 +2775,10 @@
         <v>46</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>54</v>
@@ -2769,10 +2790,10 @@
         <v>0</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K21" s="11">
         <f>'Lit review on WRF-Hydro'!G47</f>
@@ -2793,8 +2814,9 @@
       <c r="R21" s="11"/>
       <c r="S21" s="11"/>
       <c r="T21" s="11"/>
-    </row>
-    <row r="22" spans="1:20" s="2" customFormat="1" ht="49.5">
+      <c r="U21" s="11"/>
+    </row>
+    <row r="22" spans="1:21" s="2" customFormat="1" ht="49.5">
       <c r="A22" s="15" t="s">
         <v>2</v>
       </c>
@@ -2802,25 +2824,25 @@
         <v>1</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>38</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>53</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H22" s="16">
         <v>0</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J22" s="16" t="s">
         <v>19</v>
@@ -2834,15 +2856,16 @@
       <c r="M22" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="N22" s="11"/>
+      <c r="N22" s="16"/>
       <c r="O22" s="11"/>
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
       <c r="R22" s="11"/>
       <c r="S22" s="11"/>
       <c r="T22" s="11"/>
-    </row>
-    <row r="23" spans="1:20" s="2" customFormat="1" ht="297">
+      <c r="U22" s="11"/>
+    </row>
+    <row r="23" spans="1:21" s="2" customFormat="1" ht="297">
       <c r="A23" s="57" t="s">
         <v>56</v>
       </c>
@@ -2851,10 +2874,10 @@
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>54</v>
@@ -2869,7 +2892,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K23" s="11">
         <v>0.03</v>
@@ -2889,22 +2912,23 @@
       <c r="R23" s="11"/>
       <c r="S23" s="11"/>
       <c r="T23" s="11"/>
-    </row>
-    <row r="24" spans="1:20" s="2" customFormat="1" ht="66">
+      <c r="U23" s="11"/>
+    </row>
+    <row r="24" spans="1:21" s="2" customFormat="1" ht="66">
       <c r="A24" s="58"/>
       <c r="B24" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="16" t="s">
         <v>53</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H24" s="16" t="s">
         <v>19</v>
@@ -2913,10 +2937,10 @@
         <v>19</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L24" s="16" t="s">
         <v>19</v>
@@ -2924,15 +2948,16 @@
       <c r="M24" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="N24" s="11"/>
+      <c r="N24" s="16"/>
       <c r="O24" s="11"/>
       <c r="P24" s="11"/>
       <c r="Q24" s="11"/>
       <c r="R24" s="11"/>
       <c r="S24" s="11"/>
       <c r="T24" s="11"/>
-    </row>
-    <row r="25" spans="1:20" s="2" customFormat="1" ht="181.5">
+      <c r="U24" s="11"/>
+    </row>
+    <row r="25" spans="1:21" s="2" customFormat="1" ht="181.5">
       <c r="A25" s="10" t="s">
         <v>16</v>
       </c>
@@ -2950,7 +2975,7 @@
         <v>53</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>19</v>
@@ -2959,10 +2984,10 @@
         <v>19</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L25" s="16" t="s">
         <v>19</v>
@@ -2970,13 +2995,14 @@
       <c r="M25" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="N25" s="11"/>
+      <c r="N25" s="16"/>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
       <c r="Q25" s="11"/>
       <c r="R25" s="11"/>
       <c r="S25" s="11"/>
       <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1">
       <c r="A36" s="6"/>
@@ -2994,9 +3020,9 @@
   <mergeCells count="7">
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="Q1:U1"/>
     <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="J1:P1"/>
     <mergeCell ref="A3:A17"/>
     <mergeCell ref="A18:A20"/>
   </mergeCells>
@@ -3011,11 +3037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB7CFF8-16E9-44BD-BC94-406D58013BA0}">
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="1">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -3036,16 +3059,16 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="67" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="68"/>
       <c r="C1" s="68"/>
       <c r="D1" s="68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E1" s="68"/>
       <c r="F1" s="68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G1" s="68"/>
       <c r="H1" s="68"/>
@@ -3055,42 +3078,42 @@
     </row>
     <row r="2" spans="1:11" ht="66">
       <c r="A2" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>78</v>
-      </c>
       <c r="E2" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="22" t="s">
-        <v>85</v>
-      </c>
       <c r="J2" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="28" customFormat="1" ht="99">
       <c r="A3" s="66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="23" t="str">
         <f>'Definition &amp; analysis design'!B3</f>
@@ -3104,7 +3127,7 @@
         <v>57</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>19</v>
@@ -3122,7 +3145,7 @@
         <v>15</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K3" s="24"/>
     </row>
@@ -3148,7 +3171,7 @@
         <v>15</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K4" s="24"/>
     </row>
@@ -3159,19 +3182,19 @@
       <c r="D5" s="24"/>
       <c r="E5" s="24"/>
       <c r="F5" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G5" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="I5" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="H5" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>136</v>
-      </c>
       <c r="J5" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K5" s="24"/>
     </row>
@@ -3182,22 +3205,22 @@
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
       <c r="F6" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G6" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="I6" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="H6" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>136</v>
-      </c>
       <c r="J6" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="28" customFormat="1" ht="46.5" customHeight="1">
@@ -3207,7 +3230,7 @@
       <c r="D7" s="24"/>
       <c r="E7" s="24"/>
       <c r="F7" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G7" s="24" t="s">
         <v>19</v>
@@ -3219,10 +3242,10 @@
         <v>15</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="28" customFormat="1" ht="49.5">
@@ -3244,10 +3267,10 @@
         <v>11.55</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K8" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="35" customFormat="1" ht="66">
@@ -3262,13 +3285,13 @@
 [m/s]</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>35</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="33">
         <f>G10</f>
@@ -3283,7 +3306,7 @@
         <v>2.4499999999999999E-5</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K9" s="34"/>
     </row>
@@ -3307,7 +3330,7 @@
         <v>x10</v>
       </c>
       <c r="J10" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K10" s="32"/>
     </row>
@@ -3322,13 +3345,13 @@
         <v>19</v>
       </c>
       <c r="H11" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="I11" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="I11" s="32" t="s">
-        <v>149</v>
-      </c>
       <c r="J11" s="32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K11" s="32"/>
     </row>
@@ -3343,16 +3366,16 @@
         <v>19</v>
       </c>
       <c r="H12" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="I12" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="I12" s="32" t="s">
-        <v>149</v>
-      </c>
       <c r="J12" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K12" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="33">
@@ -3372,10 +3395,10 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="J13" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K13" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="49.5">
@@ -3395,7 +3418,7 @@
         <v>19</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K14" s="32"/>
     </row>
@@ -3414,7 +3437,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F15" s="24"/>
       <c r="G15" s="40">
@@ -3430,7 +3453,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K15" s="24"/>
     </row>
@@ -3454,7 +3477,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K16" s="24"/>
     </row>
@@ -3465,7 +3488,7 @@
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
       <c r="F17" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G17" s="24">
         <v>0.1</v>
@@ -3477,10 +3500,10 @@
         <v>1</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K17" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="28" customFormat="1" ht="33">
@@ -3503,10 +3526,10 @@
         <v>19</v>
       </c>
       <c r="J18" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="K18" s="24" t="s">
         <v>164</v>
-      </c>
-      <c r="K18" s="24" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="28" customFormat="1" ht="49.5">
@@ -3529,10 +3552,10 @@
         <v>19</v>
       </c>
       <c r="J19" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K19" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="132">
@@ -3550,7 +3573,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F20" s="32" t="s">
         <v>53</v>
@@ -3568,7 +3591,7 @@
         <v>0.78</v>
       </c>
       <c r="J20" s="31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K20" s="32"/>
     </row>
@@ -3589,10 +3612,10 @@
         <v>0.78</v>
       </c>
       <c r="J21" s="36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K21" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="49.5">
@@ -3612,10 +3635,10 @@
         <v>0.75900000000000001</v>
       </c>
       <c r="J22" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K22" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="28" customFormat="1" ht="82.5">
@@ -3636,7 +3659,7 @@
         <v>40</v>
       </c>
       <c r="F23" s="43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G23" s="43">
         <v>0.56999999999999995</v>
@@ -3648,7 +3671,7 @@
         <v>0.7</v>
       </c>
       <c r="J23" s="43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K23" s="43" t="s">
         <v>55</v>
@@ -3675,7 +3698,7 @@
         <v>53</v>
       </c>
       <c r="G24" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H24" s="45">
         <v>0</v>
@@ -3684,10 +3707,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="K24" s="45" t="s">
         <v>70</v>
-      </c>
-      <c r="K24" s="45" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="28" customFormat="1" ht="49.5">
@@ -3701,7 +3724,7 @@
         <v>-</v>
       </c>
       <c r="D25" s="43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E25" s="43" t="s">
         <v>19</v>
@@ -3720,7 +3743,7 @@
         <v>-1</v>
       </c>
       <c r="J25" s="43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K25" s="43" t="s">
         <v>19</v>
@@ -3757,7 +3780,7 @@
         <v>10000</v>
       </c>
       <c r="J26" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K26" s="32"/>
     </row>
@@ -3768,7 +3791,7 @@
       <c r="D27" s="32"/>
       <c r="E27" s="32"/>
       <c r="F27" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G27" s="32">
         <v>1000</v>
@@ -3780,10 +3803,10 @@
         <v>10000</v>
       </c>
       <c r="J27" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K27" s="32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="33">
@@ -3805,7 +3828,7 @@
         <v>10000</v>
       </c>
       <c r="J28" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K28" s="32"/>
     </row>
@@ -3840,7 +3863,7 @@
         <v>1.2</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K29" s="24"/>
     </row>
@@ -3865,10 +3888,10 @@
         <v>19</v>
       </c>
       <c r="J30" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K30" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="28" customFormat="1">
@@ -3892,10 +3915,10 @@
         <v>1.2</v>
       </c>
       <c r="J31" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K31" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="46" customFormat="1" ht="49.5">
@@ -3909,28 +3932,28 @@
         <v>-</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E32" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G32" s="32">
         <f>AVERAGE(H32:I32)</f>
-        <v>0.27777777777777779</v>
+        <v>0.625</v>
       </c>
       <c r="H32" s="32">
         <f>H33</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="I32" s="32">
         <f>I33</f>
-        <v>0.55555555555555558</v>
+        <v>1</v>
       </c>
       <c r="J32" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K32" s="36"/>
     </row>
@@ -3949,14 +3972,14 @@
         <v>19</v>
       </c>
       <c r="H33" s="32">
-        <v>0</v>
+        <f>0.3/1.2</f>
+        <v>0.25</v>
       </c>
       <c r="I33" s="47">
-        <f>0.5/0.9</f>
-        <v>0.55555555555555558</v>
+        <v>1</v>
       </c>
       <c r="J33" s="32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K33" s="36"/>
     </row>
@@ -3966,30 +3989,30 @@
       <c r="C34" s="45"/>
       <c r="D34" s="45"/>
       <c r="E34" s="45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F34" s="45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G34" s="45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H34" s="45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I34" s="45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J34" s="32" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K34" s="36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="28" customFormat="1" ht="82.5">
       <c r="A35" s="66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B35" s="23" t="str">
         <f>'Definition &amp; analysis design'!B18</f>
@@ -4001,28 +4024,28 @@
 [m]</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F35" s="24" t="s">
         <v>19</v>
       </c>
       <c r="G35" s="24">
-        <f>G37/1000</f>
-        <v>0.05</v>
+        <f>G37</f>
+        <v>50</v>
       </c>
       <c r="H35" s="24">
-        <f>H38/1000</f>
-        <v>0.01</v>
+        <f>H38</f>
+        <v>10</v>
       </c>
       <c r="I35" s="24">
-        <f>I38/1000</f>
-        <v>0.25</v>
+        <f>I38</f>
+        <v>250</v>
       </c>
       <c r="J35" s="48" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K35" s="24"/>
     </row>
@@ -4032,7 +4055,7 @@
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
       <c r="E36" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F36" s="24" t="s">
         <v>19</v>
@@ -4047,7 +4070,7 @@
         <v>250</v>
       </c>
       <c r="J36" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K36" s="29"/>
     </row>
@@ -4057,7 +4080,7 @@
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
       <c r="E37" s="24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F37" s="24" t="s">
         <v>19</v>
@@ -4072,10 +4095,10 @@
         <v>19</v>
       </c>
       <c r="J37" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K37" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="28" customFormat="1" ht="82.5">
@@ -4084,10 +4107,10 @@
       <c r="C38" s="24"/>
       <c r="D38" s="24"/>
       <c r="E38" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G38" s="24">
         <v>25</v>
@@ -4099,10 +4122,10 @@
         <v>250</v>
       </c>
       <c r="J38" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K38" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="28" customFormat="1" ht="82.5">
@@ -4111,7 +4134,7 @@
       <c r="C39" s="24"/>
       <c r="D39" s="24"/>
       <c r="E39" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F39" s="24" t="s">
         <v>19</v>
@@ -4126,7 +4149,7 @@
         <v>2.5</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K39" s="29"/>
     </row>
@@ -4163,7 +4186,7 @@
         <v>2</v>
       </c>
       <c r="J40" s="50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K40" s="32" t="s">
         <v>19</v>
@@ -4180,13 +4203,13 @@
         <v>19</v>
       </c>
       <c r="H41" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I41" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="J41" s="32" t="s">
         <v>144</v>
-      </c>
-      <c r="J41" s="32" t="s">
-        <v>145</v>
       </c>
       <c r="K41" s="32"/>
     </row>
@@ -4209,10 +4232,10 @@
         <v>19</v>
       </c>
       <c r="J42" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K42" s="38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -4234,7 +4257,7 @@
         <v>0.3</v>
       </c>
       <c r="J43" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K43" s="32"/>
     </row>
@@ -4270,7 +4293,7 @@
         <v>8</v>
       </c>
       <c r="J44" s="24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K44" s="24"/>
     </row>
@@ -4280,10 +4303,10 @@
       <c r="C45" s="24"/>
       <c r="D45" s="24"/>
       <c r="E45" s="24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G45" s="24">
         <v>1.75</v>
@@ -4295,10 +4318,10 @@
         <v>8</v>
       </c>
       <c r="J45" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K45" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="28" customFormat="1" ht="33">
@@ -4318,15 +4341,15 @@
         <v>19</v>
       </c>
       <c r="J46" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K46" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="63" customHeight="1">
       <c r="A47" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B47" s="31" t="str">
         <f>'Definition &amp; analysis design'!B21</f>
@@ -4356,7 +4379,7 @@
         <v>4</v>
       </c>
       <c r="J47" s="50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K47" s="32"/>
     </row>
@@ -4366,10 +4389,10 @@
       <c r="C48" s="32"/>
       <c r="D48" s="32"/>
       <c r="E48" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="F48" s="32" t="s">
         <v>204</v>
-      </c>
-      <c r="F48" s="32" t="s">
-        <v>205</v>
       </c>
       <c r="G48" s="32">
         <v>0.6</v>
@@ -4381,10 +4404,10 @@
         <v>4</v>
       </c>
       <c r="J48" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K48" s="53" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:19" ht="115.5">
@@ -4424,7 +4447,7 @@
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F50" s="24" t="s">
         <v>53</v>
@@ -4435,17 +4458,17 @@
       <c r="H50" s="24">
         <v>0</v>
       </c>
-      <c r="I50" s="24" t="s">
-        <v>58</v>
+      <c r="I50" s="24">
+        <v>1</v>
       </c>
       <c r="J50" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K50" s="24"/>
     </row>
     <row r="51" spans="1:19" s="51" customFormat="1" ht="16.5">
       <c r="A51" s="66" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B51" s="31" t="s">
         <v>33</v>

</xml_diff>